<commit_message>
Document Reorganized 2nd Time
</commit_message>
<xml_diff>
--- a/Computer Store Documents/Requirements.xlsx
+++ b/Computer Store Documents/Requirements.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Desktop\work\work\work\ComputerStore\old2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Visual Studio 2013\Projects\ComputerStore\Computer Store Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>User must be able to login successfully</t>
   </si>
@@ -217,13 +217,16 @@
   </si>
   <si>
     <t>Products</t>
+  </si>
+  <si>
+    <t>Req. No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +238,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,6 +266,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="13"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -262,13 +274,14 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,8 +299,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -306,6 +324,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -351,59 +384,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -705,91 +756,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="A1:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -800,106 +879,132 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:B12"/>
+      <selection activeCell="C12" sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="86.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -907,85 +1012,114 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A1:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -993,97 +1127,132 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C12" sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="9"/>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1091,120 +1260,167 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A1:B16"/>
+      <selection activeCell="C16" sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.5703125" style="4" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="57.5703125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7"/>
-    </row>
-    <row r="5" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="7"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1213,85 +1429,114 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="A1:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="11.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="56" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>